<commit_message>
began completing time entries for individual trials
</commit_message>
<xml_diff>
--- a/data/individual_trial_data.xlsx
+++ b/data/individual_trial_data.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Meghan/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
     <sheet name="Template" sheetId="1" r:id="rId2"/>
     <sheet name="Variable explanations" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -264,7 +272,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm:ss.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -321,6 +329,11 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF303336"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="4">
@@ -418,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -449,6 +462,7 @@
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -456,6 +470,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -781,13 +800,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.5" style="18" customWidth="1"/>
     <col min="2" max="6" width="10.83203125" style="17"/>
@@ -796,7 +815,7 @@
     <col min="10" max="10" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
@@ -833,8 +852,9 @@
       <c r="L1" s="23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="24"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="18" t="s">
         <v>77</v>
       </c>
@@ -852,377 +872,377 @@
         <v>5.617</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A41" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A42" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A43" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A44" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A45" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A46" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A47" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A48" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A66" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A68" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A70" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A71" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A72" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A73" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A74" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A75" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A76" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A77" s="18" t="s">
         <v>77</v>
       </c>
@@ -1230,11 +1250,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1251,12 +1266,12 @@
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="9" max="9" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1284,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1282,7 +1297,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1295,7 +1310,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1327,7 +1342,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1359,7 +1374,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1391,7 +1406,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1423,7 +1438,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1455,7 +1470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1487,7 +1502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1519,7 +1534,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1551,7 +1566,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -1583,7 +1598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1615,7 +1630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1647,7 +1662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1679,7 +1694,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1711,7 +1726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1743,7 +1758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1775,7 +1790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -1807,7 +1822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1839,7 +1854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -1871,7 +1886,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
@@ -1903,7 +1918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -1935,7 +1950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1967,7 +1982,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -1999,7 +2014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -2031,7 +2046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
@@ -2063,7 +2078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -2095,7 +2110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
@@ -2127,7 +2142,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -2159,7 +2174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>46</v>
       </c>
@@ -2191,7 +2206,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -2223,7 +2238,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
@@ -2255,7 +2270,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>46</v>
       </c>
@@ -2287,7 +2302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -2319,7 +2334,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
@@ -2351,7 +2366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -2383,7 +2398,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -2415,7 +2430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -2447,7 +2462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -2483,11 +2498,6 @@
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2503,13 +2513,13 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1SqUJIwvswVa2-8W_ijJBIO2NE9AR7FI1Q9DT15vWlZE/edit?usp=sharing","GENERAL NOTE: please refer to the upload instructions for the most up to date version")</f>
         <v>GENERAL NOTE: please refer to the upload instructions for the most up to date version</v>
@@ -2518,13 +2528,13 @@
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -2538,7 +2548,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2552,7 +2562,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2566,7 +2576,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2580,7 +2590,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2594,7 +2604,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2608,7 +2618,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2622,7 +2632,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2636,7 +2646,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -2650,7 +2660,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -2664,24 +2674,19 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="14"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="14"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>